<commit_message>
Checklist Qualidade e Cronograma finalizados
</commit_message>
<xml_diff>
--- a/Projeto/Documentação Apoio/Cronograma.xlsx
+++ b/Projeto/Documentação Apoio/Cronograma.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
   <si>
     <t>DESCRIÇÃO</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Analisar Incosistencia nos Requisitos</t>
   </si>
   <si>
-    <t>Checklist Inconsistência.docx</t>
-  </si>
-  <si>
     <t>Rastreabilidade</t>
   </si>
   <si>
@@ -75,16 +72,109 @@
     <t>Gerente de Configuração (Matheus F.)</t>
   </si>
   <si>
-    <t xml:space="preserve">Gerente de Requisitos (Rogério A.), Analistas (Luiz E. , Thiago N.) </t>
-  </si>
-  <si>
     <t>Gerente de Requisitos (Rogério A.)</t>
   </si>
   <si>
-    <t>Gerente de Requisitos (Rogério A.), Analistas (Luiz E. , Thiago N.)</t>
-  </si>
-  <si>
     <t>Documento de Requisitos.docx</t>
+  </si>
+  <si>
+    <t>Checklist Inconsistência.xlsx</t>
+  </si>
+  <si>
+    <t>Gerar Validação de Requisitos</t>
+  </si>
+  <si>
+    <t>Comprometimento da Equipe Técnica aos Requisitos.docx</t>
+  </si>
+  <si>
+    <t>Gerar Comprometimento da Equipe</t>
+  </si>
+  <si>
+    <t>Comprometimento Equipe</t>
+  </si>
+  <si>
+    <t>Validação com Forcedor</t>
+  </si>
+  <si>
+    <t>Validação de Requisitos.docx</t>
+  </si>
+  <si>
+    <t>Avaliação de Processo</t>
+  </si>
+  <si>
+    <t>Avaliar Processo do Software</t>
+  </si>
+  <si>
+    <t>Gerente de Qualidade (Marcus T)</t>
+  </si>
+  <si>
+    <t>Checklist Qualidade.xlsx</t>
+  </si>
+  <si>
+    <t>Travar Baseline</t>
+  </si>
+  <si>
+    <t>Gerar e Bloquear a Baseline</t>
+  </si>
+  <si>
+    <t>Gerente do Projeto (Matheus F)</t>
+  </si>
+  <si>
+    <t>Baseline.docx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ações Corretivas* </t>
+  </si>
+  <si>
+    <t>Andamento das Ações Corretivas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acompanhar Tratamento* </t>
+  </si>
+  <si>
+    <t>Ações para Corrigir Não Confirmidades</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ger. Requisitos (Rogério A.), Analistas (Luiz E. , Thiago N.) </t>
+  </si>
+  <si>
+    <t>Ger. Requisitos (Rogério A.), Analistas (Luiz E. , Thiago N.)</t>
+  </si>
+  <si>
+    <t>Gerente Responsável</t>
+  </si>
+  <si>
+    <t>Não Conformidade.docx</t>
+  </si>
+  <si>
+    <t>Ações Corretivas.docx</t>
+  </si>
+  <si>
+    <t>Documentar Não Conformidade</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Não Conformidade*</t>
+  </si>
+  <si>
+    <t>Encerrar Não conformidades</t>
+  </si>
+  <si>
+    <t>Registrar Conclusão*</t>
+  </si>
+  <si>
+    <t>Conclusão de um Ação Corretiva.docx</t>
+  </si>
+  <si>
+    <t>Finalizar Projeto</t>
+  </si>
+  <si>
+    <t>Encerrar Projeto</t>
+  </si>
+  <si>
+    <t>GYN SOLUTION</t>
+  </si>
+  <si>
+    <t>* Caso Haja Necessidade</t>
   </si>
 </sst>
 </file>
@@ -108,7 +198,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -127,6 +217,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -140,7 +242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -155,6 +257,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -437,20 +545,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.85546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="32.5703125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="58.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="36.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="52.28515625" style="3" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" style="3" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="31.28515625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="52.140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -461,7 +569,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -481,7 +589,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2" s="4">
         <v>43050</v>
@@ -501,16 +609,16 @@
         <v>9</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="D3" s="5">
         <v>43049</v>
       </c>
       <c r="E3" s="5">
-        <v>43053</v>
+        <v>43057</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -521,69 +629,222 @@
         <v>11</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="4">
+        <v>43057</v>
+      </c>
+      <c r="E4" s="4">
+        <v>43058</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="D4" s="4">
-        <v>43053</v>
-      </c>
-      <c r="E4" s="4">
-        <v>43054</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="5">
+        <v>43058</v>
+      </c>
+      <c r="E5" s="5">
+        <v>43058</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="3" t="s">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="4">
+        <v>43059</v>
+      </c>
+      <c r="E6" s="4">
+        <v>43060</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="5">
-        <v>43054</v>
-      </c>
-      <c r="E5" s="5">
-        <v>43054</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="C7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="5">
+        <v>43060</v>
+      </c>
+      <c r="E7" s="5">
+        <v>43061</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="A8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="4">
+        <v>43061</v>
+      </c>
+      <c r="E8" s="4">
+        <v>43061</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="5">
+        <v>43061</v>
+      </c>
+      <c r="E9" s="5">
+        <v>43061</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="A10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="4">
+        <v>43061</v>
+      </c>
+      <c r="E10" s="4">
+        <v>43061</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="5">
+        <v>43061</v>
+      </c>
+      <c r="E11" s="5">
+        <v>43063</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="A12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="4">
+        <v>43061</v>
+      </c>
+      <c r="E12" s="4">
+        <v>43063</v>
+      </c>
       <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="5">
+        <v>43063</v>
+      </c>
+      <c r="E13" s="5">
+        <v>43063</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="4">
+        <v>43063</v>
+      </c>
+      <c r="E14" s="4">
+        <v>43063</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>